<commit_message>
Just opened it. not change.
</commit_message>
<xml_diff>
--- a/Calc/Prices_calc.xlsx
+++ b/Calc/Prices_calc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C7D40A-7CB9-463F-9F35-21E3D4836E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>

</xml_diff>